<commit_message>
Added MasterCollection, combined CcliTop100.
</commit_message>
<xml_diff>
--- a/WorshipCreator.TestData/Source/Books/ShaneAndShane/Shane & Shane (from website) V2.xlsx
+++ b/WorshipCreator.TestData/Source/Books/ShaneAndShane/Shane & Shane (from website) V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PageOptimizer\Data\WorshipCreator.TestData\Source\Books\ShaneAndShane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB7C111-6218-43E8-B242-FF9AF0408A7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27C7B31-B8DF-475B-B666-102BB3A9F51A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1898BBCD-4A5D-4B3F-9317-061045B18130}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="806">
   <si>
     <t>G</t>
   </si>
@@ -2866,10 +2866,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B95710C-65C8-40EA-B639-B1B45687620A}">
   <dimension ref="A1:W317"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C234" sqref="C234"/>
+      <selection pane="bottomLeft" activeCell="W1" sqref="W1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13070,9 +13070,6 @@
       </c>
       <c r="K191" s="9">
         <v>7011451</v>
-      </c>
-      <c r="N191" t="s">
-        <v>709</v>
       </c>
       <c r="W191" s="1" t="str">
         <f>IF(K191=T191,"Yes","")</f>
@@ -19067,7 +19064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E7DA4D-EA9F-4757-96C7-EECDFE083310}">
   <dimension ref="A1:C217"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A193" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>